<commit_message>
add us ip 32-54
</commit_message>
<xml_diff>
--- a/xls/cfips.xlsx
+++ b/xls/cfips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhq\PycharmProjects\cfip\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B458BD5-1E7A-4153-B6C7-BBBD718D36CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEA9F7C-F2D7-4EFA-B316-B12940239A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="26136" windowHeight="16776" xr2:uid="{49388C81-6084-40E2-9286-EB25114461FB}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="109">
   <si>
     <t>IP</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -294,6 +294,75 @@
   </si>
   <si>
     <t>154.23.207.16</t>
+  </si>
+  <si>
+    <t>47.88.15.127</t>
+  </si>
+  <si>
+    <t>129.159.84.71</t>
+  </si>
+  <si>
+    <t>152.67.231.219</t>
+  </si>
+  <si>
+    <t>193.122.197.111</t>
+  </si>
+  <si>
+    <t>150.136.61.148</t>
+  </si>
+  <si>
+    <t>192.9.159.65</t>
+  </si>
+  <si>
+    <t>47.90.141.204</t>
+  </si>
+  <si>
+    <t>129.80.116.250</t>
+  </si>
+  <si>
+    <t>129.146.254.39</t>
+  </si>
+  <si>
+    <t>192.18.143.199</t>
+  </si>
+  <si>
+    <t>47.253.56.77</t>
+  </si>
+  <si>
+    <t>155.248.196.123</t>
+  </si>
+  <si>
+    <t>192.9.250.241</t>
+  </si>
+  <si>
+    <t>132.145.134.230</t>
+  </si>
+  <si>
+    <t>192.9.138.241</t>
+  </si>
+  <si>
+    <t>47.253.105.131</t>
+  </si>
+  <si>
+    <t>47.89.244.253</t>
+  </si>
+  <si>
+    <t>150.230.47.17</t>
+  </si>
+  <si>
+    <t>164.152.17.14</t>
+  </si>
+  <si>
+    <t>129.146.243.241</t>
+  </si>
+  <si>
+    <t>152.70.155.147</t>
+  </si>
+  <si>
+    <t>129.146.248.140</t>
+  </si>
+  <si>
+    <t>132.145.152.194</t>
   </si>
 </sst>
 </file>
@@ -660,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A2EC68-E687-4E9E-A956-08081462728F}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G2:G32"/>
+      <selection activeCell="G55" sqref="G2:G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1290,7 +1359,7 @@
         <v>34</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" ref="F25:F32" si="6">ROW()-1</f>
+        <f t="shared" ref="F25:F55" si="6">ROW()-1</f>
         <v>24</v>
       </c>
       <c r="G25" t="str">
@@ -1455,7 +1524,7 @@
       <c r="B32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>443</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1473,35 +1542,580 @@
         <v>27.50.48.108:443#US_31</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="D36"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1">
+        <v>443</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" ref="G33:G55" si="8">A33&amp;B33&amp;C33&amp;D33&amp;E33&amp;"_"&amp;F33</f>
+        <v>47.88.15.127:443#US_32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1">
+        <v>443</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="6"/>
+        <v>33</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="8"/>
+        <v>129.159.84.71:443#US_33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="1">
+        <v>443</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="6"/>
+        <v>34</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="8"/>
+        <v>152.67.231.219:443#US_34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1">
+        <v>443</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="8"/>
+        <v>193.122.197.111:443#US_35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1">
+        <v>443</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="6"/>
+        <v>36</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="8"/>
+        <v>150.136.61.148:443#US_36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="1">
+        <v>443</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="6"/>
+        <v>37</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="8"/>
+        <v>192.9.159.65:443#US_37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1">
+        <v>443</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="6"/>
+        <v>38</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="8"/>
+        <v>47.90.141.204:443#US_38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1">
+        <v>443</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="6"/>
+        <v>39</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="8"/>
+        <v>129.80.116.250:443#US_39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="1">
+        <v>443</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="8"/>
+        <v>129.146.254.39:443#US_40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="1">
+        <v>443</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="6"/>
+        <v>41</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="8"/>
+        <v>192.18.143.199:443#US_41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="1">
+        <v>443</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="6"/>
+        <v>42</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="8"/>
+        <v>47.253.56.77:443#US_42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="1">
+        <v>443</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="6"/>
+        <v>43</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="8"/>
+        <v>155.248.196.123:443#US_43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1">
+        <v>443</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="6"/>
+        <v>44</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="8"/>
+        <v>192.9.250.241:443#US_44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1">
+        <v>443</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="8"/>
+        <v>132.145.134.230:443#US_45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="1">
+        <v>443</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="6"/>
+        <v>46</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="8"/>
+        <v>192.9.138.241:443#US_46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="1">
+        <v>443</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="6"/>
+        <v>47</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="8"/>
+        <v>47.253.105.131:443#US_47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="1">
+        <v>443</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="6"/>
+        <v>48</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="8"/>
+        <v>47.89.244.253:443#US_48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="1">
+        <v>443</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="6"/>
+        <v>49</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="8"/>
+        <v>150.230.47.17:443#US_49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="1">
+        <v>443</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="8"/>
+        <v>164.152.17.14:443#US_50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="1">
+        <v>443</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="6"/>
+        <v>51</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="8"/>
+        <v>129.146.243.241:443#US_51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="1">
+        <v>443</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="6"/>
+        <v>52</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="8"/>
+        <v>152.70.155.147:443#US_52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="1">
+        <v>443</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="6"/>
+        <v>53</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="8"/>
+        <v>129.146.248.140:443#US_53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="1">
+        <v>443</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="6"/>
+        <v>54</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="8"/>
+        <v>132.145.152.194:443#US_54</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G32">

</xml_diff>